<commit_message>
Am modificat plot-urile de Fabrication și am actualizat Excel-ul cu BOM-ul - verificat dacă am primit componentele corecte. Am descoperit mai multe probleme pe placă. Probabil o să trebuiască să creez o variantă nouă.
</commit_message>
<xml_diff>
--- a/01 BOM/8307_BOM.xlsx
+++ b/01 BOM/8307_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/KiCAD/8307/01 BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/KiCAD/00 Proiecte/8307 RF Power Sensor Rev1/01 BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAA710E-CF35-AD41-92D4-FF01BD72475B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788828A0-FD92-2440-B00D-C72FC0B576AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>Id</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>611-JS102011SAQN</t>
+  </si>
+  <si>
+    <t>Check dacă le am</t>
+  </si>
+  <si>
+    <t>da</t>
   </si>
 </sst>
 </file>
@@ -780,13 +786,20 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1143,22 +1156,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="67.33203125" customWidth="1"/>
     <col min="5" max="5" width="37.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1174,14 +1188,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1197,14 +1214,17 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1220,14 +1240,17 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1243,14 +1266,17 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1266,11 +1292,11 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1283,17 +1309,20 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>220</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1306,17 +1335,20 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>110</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1329,17 +1361,20 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>22</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1352,17 +1387,20 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>470</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1375,20 +1413,23 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>53</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1401,20 +1442,23 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>61</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1427,20 +1471,23 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>248</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="2">
         <v>249</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1456,14 +1503,17 @@
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1480,7 +1530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1496,17 +1546,17 @@
       <c r="E15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1523,7 +1573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1539,17 +1589,17 @@
       <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1565,14 +1615,17 @@
       <c r="E18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1588,11 +1641,11 @@
       <c r="E19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1608,11 +1661,11 @@
       <c r="E20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1628,14 +1681,17 @@
       <c r="E21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1651,14 +1707,14 @@
       <c r="E22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1674,14 +1730,14 @@
       <c r="E23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1697,48 +1753,48 @@
       <c r="E24" t="s">
         <v>56</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F15" r:id="rId1" display="https://ro.mouser.com/ProductDetail/571-2118728-2" xr:uid="{C99A9A41-27D3-794C-9175-7B53F81B294F}"/>
-    <hyperlink ref="G15" r:id="rId2" display="https://ro.mouser.com/ProductDetail/571-2118727-2" xr:uid="{162EF200-04E3-E14D-BFA6-B2A18D6A1AC3}"/>
-    <hyperlink ref="G22" r:id="rId3" display="https://ro.mouser.com/ProductDetail/584-LT1117IST-5%23PBF" xr:uid="{37CF12C1-DEE0-9248-A68D-715364B033C0}"/>
-    <hyperlink ref="G21" r:id="rId4" display="https://ro.mouser.com/ProductDetail/994-1206CS-060XJLB" xr:uid="{BEEEB196-A212-BE49-BAAB-D6120316CF50}"/>
-    <hyperlink ref="G9" r:id="rId5" display="https://ro.mouser.com/ProductDetail/660-SG73G1JTTD4700D" xr:uid="{3AC9C6CD-31FC-8046-85DA-BE918EA104AE}"/>
-    <hyperlink ref="G8" r:id="rId6" display="https://ro.mouser.com/ProductDetail/660-SG73G1JTTD22R0D" xr:uid="{F4BD4924-C0FE-8845-9844-7AE7F3C24FB3}"/>
-    <hyperlink ref="G6" r:id="rId7" display="https://ro.mouser.com/ProductDetail/660-SG73G1JTTD2200D" xr:uid="{5A384645-D964-C942-AD66-7F2846445233}"/>
-    <hyperlink ref="G11" r:id="rId8" display="https://ro.mouser.com/ProductDetail/71-CRCW060360R4FKEAC" xr:uid="{9DFD9D93-943F-1F48-82F7-1501421C9194}"/>
-    <hyperlink ref="G12" r:id="rId9" display="https://ro.mouser.com/ProductDetail/603-AT0603BRD07249RL" xr:uid="{3D5A2DF8-CB3A-DF49-A3D0-6F3F9D14F330}"/>
-    <hyperlink ref="G10" r:id="rId10" display="https://ro.mouser.com/ProductDetail/603-RC0603FR-0753R6L" xr:uid="{0F306E03-B303-AB43-BCDD-5D8BF8EB797D}"/>
-    <hyperlink ref="G7" r:id="rId11" display="https://ro.mouser.com/ProductDetail/603-RT0603DRD07110RL" xr:uid="{0A564324-CBFF-A34F-A1E8-F746A6C929AC}"/>
-    <hyperlink ref="G13" r:id="rId12" display="https://ro.mouser.com/ProductDetail/710-885012206020" xr:uid="{30B0798E-7D1F-0E44-852D-0E7AF0539B60}"/>
-    <hyperlink ref="G2" r:id="rId13" display="https://ro.mouser.com/ProductDetail/710-885012006003" xr:uid="{AD51C09C-748E-044D-AEC3-5B856C705101}"/>
-    <hyperlink ref="G3" r:id="rId14" display="https://ro.mouser.com/ProductDetail/603-CC603KRX7R6BB103" xr:uid="{5CD302DD-92D0-5349-A69E-ED353FC92E88}"/>
-    <hyperlink ref="G4" r:id="rId15" display="https://ro.mouser.com/ProductDetail/710-885012206008" xr:uid="{7835FA02-76D6-CD45-BBCA-061E2A1B4100}"/>
-    <hyperlink ref="G18" r:id="rId16" display="https://ro.mouser.com/ProductDetail/647-UWT1C100MCL2B" xr:uid="{71592315-37E2-0744-B37D-A21E8B20DE74}"/>
-    <hyperlink ref="G17" r:id="rId17" display="https://ro.mouser.com/ProductDetail/647-UWT1C100MCL2B" xr:uid="{7BCBBBA1-8021-EC42-BE9F-AE955036FD46}"/>
-    <hyperlink ref="G23" r:id="rId18" display="https://ro.mouser.com/ProductDetail/584-AD8307ARZ" xr:uid="{C7D2FC1F-6842-774A-956E-8A91A0A0E96D}"/>
-    <hyperlink ref="H2" r:id="rId19" xr:uid="{817DCD5A-91EA-4744-9D52-FE6D85AE09B2}"/>
-    <hyperlink ref="H3" r:id="rId20" xr:uid="{D00009E3-3477-EE46-87B5-DD3C519C82FF}"/>
-    <hyperlink ref="H4" r:id="rId21" xr:uid="{C9736EE3-5612-C548-B9A0-2A2A19C1180E}"/>
-    <hyperlink ref="H6" r:id="rId22" xr:uid="{9D763616-5E9F-6D4F-9D0E-1425892F7766}"/>
-    <hyperlink ref="H7" r:id="rId23" xr:uid="{67CAC842-F2B1-7D4C-9331-95563748383A}"/>
-    <hyperlink ref="H8" r:id="rId24" xr:uid="{41228FAC-61E5-5845-A622-BC91F29F6999}"/>
-    <hyperlink ref="H9" r:id="rId25" xr:uid="{65304B93-539B-154A-BD52-AE2F60AAEE27}"/>
-    <hyperlink ref="H10" r:id="rId26" xr:uid="{0BDBF4B2-3B7E-8540-864B-7DA44BFD99F7}"/>
-    <hyperlink ref="H11" r:id="rId27" xr:uid="{54FC4982-C7BE-A442-BF7F-263D50448A52}"/>
-    <hyperlink ref="H12" r:id="rId28" xr:uid="{FB4D9ACF-80BC-F149-AD97-B78E13E14CA1}"/>
-    <hyperlink ref="H13" r:id="rId29" xr:uid="{B5098BE7-83A3-6447-9E0E-C3D00709D6E5}"/>
-    <hyperlink ref="H15" r:id="rId30" xr:uid="{BC95EB99-321C-9144-9701-CA26DC6733B6}"/>
-    <hyperlink ref="H17" r:id="rId31" xr:uid="{2970C500-AE67-4042-B437-9753FB3ACD32}"/>
-    <hyperlink ref="H18" r:id="rId32" xr:uid="{52AFC79F-0334-FB40-9ABF-F93E7403F69A}"/>
-    <hyperlink ref="H21" r:id="rId33" xr:uid="{6B48C0F5-4037-024A-A3B7-DB1322932A13}"/>
-    <hyperlink ref="H22" r:id="rId34" xr:uid="{6EAF2CD3-DF70-4A4D-9762-DDD3CFC37ED8}"/>
-    <hyperlink ref="H23" r:id="rId35" xr:uid="{E41AC182-D03D-4C42-B1AC-8E9264D487CE}"/>
-    <hyperlink ref="G20" r:id="rId36" xr:uid="{272E2E32-5C40-F442-B9A2-45DE53CECC81}"/>
+    <hyperlink ref="G15" r:id="rId1" display="https://ro.mouser.com/ProductDetail/571-2118728-2" xr:uid="{C99A9A41-27D3-794C-9175-7B53F81B294F}"/>
+    <hyperlink ref="H15" r:id="rId2" display="https://ro.mouser.com/ProductDetail/571-2118727-2" xr:uid="{162EF200-04E3-E14D-BFA6-B2A18D6A1AC3}"/>
+    <hyperlink ref="H22" r:id="rId3" display="https://ro.mouser.com/ProductDetail/584-LT1117IST-5%23PBF" xr:uid="{37CF12C1-DEE0-9248-A68D-715364B033C0}"/>
+    <hyperlink ref="H21" r:id="rId4" display="https://ro.mouser.com/ProductDetail/994-1206CS-060XJLB" xr:uid="{BEEEB196-A212-BE49-BAAB-D6120316CF50}"/>
+    <hyperlink ref="H9" r:id="rId5" display="https://ro.mouser.com/ProductDetail/660-SG73G1JTTD4700D" xr:uid="{3AC9C6CD-31FC-8046-85DA-BE918EA104AE}"/>
+    <hyperlink ref="H8" r:id="rId6" display="https://ro.mouser.com/ProductDetail/660-SG73G1JTTD22R0D" xr:uid="{F4BD4924-C0FE-8845-9844-7AE7F3C24FB3}"/>
+    <hyperlink ref="H6" r:id="rId7" display="https://ro.mouser.com/ProductDetail/660-SG73G1JTTD2200D" xr:uid="{5A384645-D964-C942-AD66-7F2846445233}"/>
+    <hyperlink ref="H11" r:id="rId8" display="https://ro.mouser.com/ProductDetail/71-CRCW060360R4FKEAC" xr:uid="{9DFD9D93-943F-1F48-82F7-1501421C9194}"/>
+    <hyperlink ref="H12" r:id="rId9" display="https://ro.mouser.com/ProductDetail/603-AT0603BRD07249RL" xr:uid="{3D5A2DF8-CB3A-DF49-A3D0-6F3F9D14F330}"/>
+    <hyperlink ref="H10" r:id="rId10" display="https://ro.mouser.com/ProductDetail/603-RC0603FR-0753R6L" xr:uid="{0F306E03-B303-AB43-BCDD-5D8BF8EB797D}"/>
+    <hyperlink ref="H7" r:id="rId11" display="https://ro.mouser.com/ProductDetail/603-RT0603DRD07110RL" xr:uid="{0A564324-CBFF-A34F-A1E8-F746A6C929AC}"/>
+    <hyperlink ref="H13" r:id="rId12" display="https://ro.mouser.com/ProductDetail/710-885012206020" xr:uid="{30B0798E-7D1F-0E44-852D-0E7AF0539B60}"/>
+    <hyperlink ref="H2" r:id="rId13" display="https://ro.mouser.com/ProductDetail/710-885012006003" xr:uid="{AD51C09C-748E-044D-AEC3-5B856C705101}"/>
+    <hyperlink ref="H3" r:id="rId14" display="https://ro.mouser.com/ProductDetail/603-CC603KRX7R6BB103" xr:uid="{5CD302DD-92D0-5349-A69E-ED353FC92E88}"/>
+    <hyperlink ref="H4" r:id="rId15" display="https://ro.mouser.com/ProductDetail/710-885012206008" xr:uid="{7835FA02-76D6-CD45-BBCA-061E2A1B4100}"/>
+    <hyperlink ref="H18" r:id="rId16" display="https://ro.mouser.com/ProductDetail/647-UWT1C100MCL2B" xr:uid="{71592315-37E2-0744-B37D-A21E8B20DE74}"/>
+    <hyperlink ref="H17" r:id="rId17" display="https://ro.mouser.com/ProductDetail/647-UWT1C100MCL2B" xr:uid="{7BCBBBA1-8021-EC42-BE9F-AE955036FD46}"/>
+    <hyperlink ref="H23" r:id="rId18" display="https://ro.mouser.com/ProductDetail/584-AD8307ARZ" xr:uid="{C7D2FC1F-6842-774A-956E-8A91A0A0E96D}"/>
+    <hyperlink ref="I2" r:id="rId19" xr:uid="{817DCD5A-91EA-4744-9D52-FE6D85AE09B2}"/>
+    <hyperlink ref="I3" r:id="rId20" xr:uid="{D00009E3-3477-EE46-87B5-DD3C519C82FF}"/>
+    <hyperlink ref="I4" r:id="rId21" xr:uid="{C9736EE3-5612-C548-B9A0-2A2A19C1180E}"/>
+    <hyperlink ref="I6" r:id="rId22" xr:uid="{9D763616-5E9F-6D4F-9D0E-1425892F7766}"/>
+    <hyperlink ref="I7" r:id="rId23" xr:uid="{67CAC842-F2B1-7D4C-9331-95563748383A}"/>
+    <hyperlink ref="I8" r:id="rId24" xr:uid="{41228FAC-61E5-5845-A622-BC91F29F6999}"/>
+    <hyperlink ref="I9" r:id="rId25" xr:uid="{65304B93-539B-154A-BD52-AE2F60AAEE27}"/>
+    <hyperlink ref="I10" r:id="rId26" xr:uid="{0BDBF4B2-3B7E-8540-864B-7DA44BFD99F7}"/>
+    <hyperlink ref="I11" r:id="rId27" xr:uid="{54FC4982-C7BE-A442-BF7F-263D50448A52}"/>
+    <hyperlink ref="I12" r:id="rId28" xr:uid="{FB4D9ACF-80BC-F149-AD97-B78E13E14CA1}"/>
+    <hyperlink ref="I13" r:id="rId29" xr:uid="{B5098BE7-83A3-6447-9E0E-C3D00709D6E5}"/>
+    <hyperlink ref="I15" r:id="rId30" xr:uid="{BC95EB99-321C-9144-9701-CA26DC6733B6}"/>
+    <hyperlink ref="I17" r:id="rId31" xr:uid="{2970C500-AE67-4042-B437-9753FB3ACD32}"/>
+    <hyperlink ref="I18" r:id="rId32" xr:uid="{52AFC79F-0334-FB40-9ABF-F93E7403F69A}"/>
+    <hyperlink ref="I21" r:id="rId33" xr:uid="{6B48C0F5-4037-024A-A3B7-DB1322932A13}"/>
+    <hyperlink ref="I22" r:id="rId34" xr:uid="{6EAF2CD3-DF70-4A4D-9762-DDD3CFC37ED8}"/>
+    <hyperlink ref="I23" r:id="rId35" xr:uid="{E41AC182-D03D-4C42-B1AC-8E9264D487CE}"/>
+    <hyperlink ref="H20" r:id="rId36" xr:uid="{272E2E32-5C40-F442-B9A2-45DE53CECC81}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Am făcut sursa de documente publică (GitHub) și am modificat ceva documente; atenție, versiunea 1 are o eroare.
</commit_message>
<xml_diff>
--- a/01 BOM/8307_BOM.xlsx
+++ b/01 BOM/8307_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/KiCAD/00 Proiecte/8307 RF Power Sensor Rev1/01 BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788828A0-FD92-2440-B00D-C72FC0B576AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0828AC1D-03D0-4B4A-8E5C-7868AB3179B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>Id</t>
   </si>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1588,6 +1588,9 @@
       </c>
       <c r="E17" t="s">
         <v>37</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>39</v>

</xml_diff>